<commit_message>
Updated positions of balises in TrackDescription
</commit_message>
<xml_diff>
--- a/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
+++ b/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -591,7 +591,7 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
-        <v>24</v>
+        <v>241</v>
       </c>
       <c r="B2" s="7">
         <v>352</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
-        <v>118</v>
+        <v>1181</v>
       </c>
       <c r="B3" s="7">
         <v>353</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
-        <v>280</v>
+        <v>2801</v>
       </c>
       <c r="B12" s="7">
         <v>354</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
-        <v>361</v>
+        <v>3612</v>
       </c>
       <c r="B13" s="7">
         <v>351</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="14" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
-        <v>367</v>
+        <v>3666</v>
       </c>
       <c r="B14" s="7">
         <v>355</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
-        <v>381</v>
+        <v>3812</v>
       </c>
       <c r="B15" s="7">
         <v>356</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
-        <v>386.8</v>
+        <v>3868</v>
       </c>
       <c r="B16" s="7">
         <v>357</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
-        <v>404</v>
+        <v>4043</v>
       </c>
       <c r="B17" s="7">
         <v>358</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
-        <v>421</v>
+        <v>4215</v>
       </c>
       <c r="B18" s="7">
         <v>359</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>427</v>
+        <v>4270</v>
       </c>
       <c r="B19" s="7">
         <v>360</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
-        <v>469</v>
+        <v>4695</v>
       </c>
       <c r="B20" s="7">
         <v>361</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>475</v>
+        <v>4749</v>
       </c>
       <c r="B21" s="7">
         <v>362</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>499</v>
+        <v>4990</v>
       </c>
       <c r="B22" s="7">
         <v>363</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="23" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
-        <v>504</v>
+        <v>5044</v>
       </c>
       <c r="B23" s="5">
         <v>364</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="24" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
-        <v>521</v>
+        <v>5213</v>
       </c>
       <c r="B24" s="5">
         <v>365</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="25" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
-        <v>527</v>
+        <v>5268</v>
       </c>
       <c r="B25" s="5">
         <v>366</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="26" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
-        <v>542</v>
+        <v>5420</v>
       </c>
       <c r="B26" s="5">
         <v>367</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="27" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
-        <v>556</v>
+        <v>5564</v>
       </c>
       <c r="B27" s="5">
         <v>368</v>

</xml_diff>

<commit_message>
Fix for "Message 3: Gradient profile is missing"
refers to #647
</commit_message>
<xml_diff>
--- a/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
+++ b/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Position (m)</t>
   </si>
@@ -80,6 +80,9 @@
     <t>Acknowledgement</t>
   </si>
   <si>
+    <t>…</t>
+  </si>
+  <si>
     <t>P42 (Session Management) / P46 (Conditional Level Transition) nominal / P46 reverse / P3 (National Values)</t>
   </si>
   <si>
@@ -96,24 +99,6 @@
   </si>
   <si>
     <t>--</t>
-  </si>
-  <si>
-    <t>P57 (Movement Authority Parameter) / P58 (Position Report Parameters)</t>
-  </si>
-  <si>
-    <t>Parameter set</t>
-  </si>
-  <si>
-    <t>Position report</t>
-  </si>
-  <si>
-    <t>P0 (Position Report) / P5 (Train Running Number)</t>
-  </si>
-  <si>
-    <t>P15 (Level 2/3 Movement Authority) / P27 (International Static Speed Profile - Nominal) / P27 (International Static Speed Profile - Reverse) / P3 (National Values) / P5 (Linking) / P41 (Level Transition Order) / P65 (Temporary Speed Restriction)</t>
-  </si>
-  <si>
-    <t>Movement Authority / Level Transition order</t>
   </si>
 </sst>
 </file>
@@ -137,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +144,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFC10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -285,9 +264,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -724,217 +700,180 @@
         <v>24</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10">
-        <v>146</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>2801</v>
+      </c>
+      <c r="B12" s="7">
+        <v>354</v>
+      </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="10">
-        <v>136</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>27</v>
+      <c r="D12" s="10"/>
+      <c r="E12" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
-        <v>2801</v>
+        <v>3612</v>
       </c>
       <c r="B13" s="7">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>3666</v>
+      </c>
+      <c r="B14" s="7">
+        <v>355</v>
+      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>29</v>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
-        <v>3612</v>
+        <v>3812</v>
       </c>
       <c r="B15" s="7">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="10"/>
+      <c r="E15" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
-        <v>3666</v>
+        <v>3868</v>
       </c>
       <c r="B16" s="7">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="6" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
-        <v>3812</v>
+        <v>4043</v>
       </c>
       <c r="B17" s="7">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
-        <v>3868</v>
+        <v>4215</v>
       </c>
       <c r="B18" s="7">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>4043</v>
+        <v>4270</v>
       </c>
       <c r="B19" s="7">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
-        <v>4215</v>
+        <v>4695</v>
       </c>
       <c r="B20" s="7">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="10"/>
+      <c r="E20" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>4270</v>
+        <v>4749</v>
       </c>
       <c r="B21" s="7">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>4695</v>
+        <v>4990</v>
       </c>
       <c r="B22" s="7">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>4749</v>
-      </c>
-      <c r="B23" s="7">
-        <v>362</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>4990</v>
-      </c>
-      <c r="B24" s="7">
-        <v>363</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>5044</v>
+      </c>
+      <c r="B23" s="5">
+        <v>364</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
+        <v>5213</v>
+      </c>
+      <c r="B24" s="5">
+        <v>365</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
-        <v>5044</v>
+        <v>5268</v>
       </c>
       <c r="B25" s="5">
-        <v>364</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>23</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
-        <v>5213</v>
+        <v>5420</v>
       </c>
       <c r="B26" s="5">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
-        <v>5268</v>
+        <v>5564</v>
       </c>
       <c r="B27" s="5">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15">
-        <v>5420</v>
-      </c>
-      <c r="B28" s="5">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
-        <v>5564</v>
-      </c>
-      <c r="B29" s="5">
         <v>368</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update track description (xls)
</commit_message>
<xml_diff>
--- a/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
+++ b/model/Scade/System/TracksideDynamicModel/TestTracks/UtrechtAmsterdam_oETCS/TrackDescription.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10848"/>
   </bookViews>
   <sheets>
-    <sheet name="DebugDescription" sheetId="1" r:id="rId1"/>
+    <sheet name="BTM_RTM" sheetId="1" r:id="rId1"/>
+    <sheet name="MAs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Position (m)</t>
   </si>
@@ -99,6 +100,27 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>Train position report (periodic)</t>
+  </si>
+  <si>
+    <t>Empty general message (periodic to keep connection alive)</t>
+  </si>
+  <si>
+    <t>(3072)</t>
+  </si>
+  <si>
+    <t>P57 (Movement Authority Request Parameters) / P58 (Position Report Parameters)</t>
+  </si>
+  <si>
+    <t>P15 (Level 2/3 Movement Authority) / P21 (Gradient Profile) / P27 (International Static Speed Profile) / P3 (National Values) / P5 (Linking) / P41 (Level Transition Order) / P65 (Temporary Speed Restriction)</t>
+  </si>
+  <si>
+    <t>Movement Authority</t>
+  </si>
+  <si>
+    <t>MA Request</t>
   </si>
 </sst>
 </file>
@@ -122,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +166,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFC10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -265,6 +299,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -693,192 +736,299 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8">
         <v>24</v>
       </c>
       <c r="D10" s="10"/>
+      <c r="E10" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="10">
+        <v>146</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19">
+        <v>136</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="18">
+        <v>24</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="F15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
         <v>2801</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B17" s="7">
         <v>354</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>3612</v>
-      </c>
-      <c r="B13" s="7">
-        <v>351</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
-        <v>3666</v>
-      </c>
-      <c r="B14" s="7">
-        <v>355</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
-        <v>3812</v>
-      </c>
-      <c r="B15" s="7">
-        <v>356</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
-        <v>3868</v>
-      </c>
-      <c r="B16" s="7">
-        <v>357</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>4043</v>
-      </c>
-      <c r="B17" s="7">
-        <v>358</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>4215</v>
-      </c>
-      <c r="B18" s="7">
-        <v>359</v>
-      </c>
-      <c r="C18" s="8"/>
+      <c r="E17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8">
+        <v>3</v>
+      </c>
       <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>4270</v>
-      </c>
-      <c r="B19" s="7">
-        <v>360</v>
-      </c>
+      <c r="E18" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>4695</v>
-      </c>
-      <c r="B20" s="7">
-        <v>361</v>
-      </c>
+      <c r="D19" s="10">
+        <v>146</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="10">
+        <v>132</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>4749</v>
+        <v>3612</v>
       </c>
       <c r="B21" s="7">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>4990</v>
+        <v>3666</v>
       </c>
       <c r="B22" s="7">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15">
+      <c r="E22" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>3812</v>
+      </c>
+      <c r="B23" s="7">
+        <v>356</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>3868</v>
+      </c>
+      <c r="B24" s="7">
+        <v>357</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>4043</v>
+      </c>
+      <c r="B25" s="7">
+        <v>358</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>4215</v>
+      </c>
+      <c r="B26" s="7">
+        <v>359</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>4270</v>
+      </c>
+      <c r="B27" s="7">
+        <v>360</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>4695</v>
+      </c>
+      <c r="B28" s="7">
+        <v>361</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>4749</v>
+      </c>
+      <c r="B29" s="7">
+        <v>362</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>4990</v>
+      </c>
+      <c r="B30" s="7">
+        <v>363</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
         <v>5044</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B31" s="5">
         <v>364</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E31" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15">
+    <row r="32" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
         <v>5213</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B32" s="5">
         <v>365</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15">
+    <row r="33" spans="1:2" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
         <v>5268</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B33" s="5">
         <v>366</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+    <row r="34" spans="1:2" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
         <v>5420</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B34" s="5">
         <v>367</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15">
+    <row r="35" spans="1:2" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
         <v>5564</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B35" s="5">
         <v>368</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A18" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>